<commit_message>
updated so that the SQL module converts the first column be styled as Title text (first letter of each word is capitalized). Then the entire df is sorted based on the first column. This is done so that the dataframe is sorted by text. Otherwise, upper case letters are lower on the ASCII table than lower case letters.
</commit_message>
<xml_diff>
--- a/Excel Table to SQL/Data.xlsx
+++ b/Excel Table to SQL/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\100. Projects\1. MicoProjects\Dict From Excel Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\100. Projects\1. MicoProjects\Excel Table to SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7692378B-E267-4EFE-BB5B-CD74CE6CCD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA9B1F5-EA28-499B-A8AD-EEAE8C61A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="5400" windowWidth="14895" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15450" yWindow="1335" windowWidth="14895" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1320,7 +1320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1339,20 +1339,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1363,6 +1473,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D381452-8EB2-4843-8AC4-22B3070133E0}" name="Table2" displayName="Table2" ref="A1:C502" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:C502" xr:uid="{4D381452-8EB2-4843-8AC4-22B3070133E0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DADD7F85-BB8D-4888-95A6-A4597AF86C2B}" name="CATEGORY" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FED6FCD6-273E-4BC4-B1B0-507DAFE1DD53}" name="COMMODITY" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{0568FDF4-5A19-4ECF-AAD9-A03E3A421D22}" name="SUB COMMODITY" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1631,13 +1753,13 @@
   <dimension ref="A1:C502"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7152,13 +7274,13 @@
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A502" s="2" t="s">
+      <c r="A502" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="B502" s="2" t="s">
+      <c r="B502" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C502" s="2" t="s">
+      <c r="C502" s="4" t="s">
         <v>411</v>
       </c>
     </row>
@@ -7167,6 +7289,9 @@
     <sortCondition ref="A2:A502"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>